<commit_message>
fixed getCustomerbyphone in ffscontroller
added threads
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/proj. mgt/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/proj. mgt/Iteration og faseplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="Overordnet projektplan" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="161">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -488,6 +488,21 @@
   </si>
   <si>
     <t>E2 14/5 - 18/5</t>
+  </si>
+  <si>
+    <t>Fremlæggelser på klassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opdatering af datamodel </t>
+  </si>
+  <si>
+    <t>opdatering af klassenavne</t>
+  </si>
+  <si>
+    <t>Tweaked GUI</t>
+  </si>
+  <si>
+    <t>Få tråde til at virke</t>
   </si>
 </sst>
 </file>
@@ -925,7 +940,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -936,11 +951,11 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="U4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V12" sqref="V12"/>
+      <selection pane="bottomRight" activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1255,6 +1270,9 @@
       <c r="V6" s="20" t="s">
         <v>123</v>
       </c>
+      <c r="W6" s="20" t="s">
+        <v>156</v>
+      </c>
       <c r="Z6" s="10"/>
       <c r="AB6"/>
       <c r="AC6"/>
@@ -1318,6 +1336,9 @@
       <c r="V7" t="s">
         <v>129</v>
       </c>
+      <c r="W7" t="s">
+        <v>157</v>
+      </c>
       <c r="Z7" s="10"/>
       <c r="AB7"/>
       <c r="AC7"/>
@@ -1378,6 +1399,9 @@
       <c r="V8" t="s">
         <v>128</v>
       </c>
+      <c r="W8" t="s">
+        <v>158</v>
+      </c>
       <c r="Z8" s="10"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
@@ -1440,6 +1464,9 @@
       <c r="V9" t="s">
         <v>130</v>
       </c>
+      <c r="W9" t="s">
+        <v>159</v>
+      </c>
       <c r="Z9" s="10"/>
       <c r="AB9" s="8"/>
       <c r="AC9" s="8"/>
@@ -1481,6 +1508,9 @@
       </c>
       <c r="V10" t="s">
         <v>131</v>
+      </c>
+      <c r="W10" t="s">
+        <v>160</v>
       </c>
       <c r="Z10" s="10"/>
       <c r="AB10" s="8"/>
@@ -1841,7 +1871,7 @@
   <sheetPr codeName="Ark2"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
opdateret IP/FP & UC5 beksrevet
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/proj. mgt/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/proj. mgt/Iteration og faseplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="171">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -518,6 +518,21 @@
   </si>
   <si>
     <t>tweaket GUI</t>
+  </si>
+  <si>
+    <t>opdater CD</t>
+  </si>
+  <si>
+    <t>implementer UC4</t>
+  </si>
+  <si>
+    <t>mockups til UC 4</t>
+  </si>
+  <si>
+    <t>UC5 beskrevet</t>
+  </si>
+  <si>
+    <t>implementation af UC5</t>
   </si>
 </sst>
 </file>
@@ -967,10 +982,10 @@
   <dimension ref="A1:AH44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="V4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Y10" sqref="Y10"/>
+      <selection pane="bottomRight" activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1122,10 +1137,10 @@
         <v>43242</v>
       </c>
       <c r="Z3" s="3">
-        <v>43242</v>
+        <v>43243</v>
       </c>
       <c r="AA3" s="3">
-        <v>43243</v>
+        <v>43244</v>
       </c>
       <c r="AB3" s="3">
         <v>43244</v>
@@ -1295,7 +1310,12 @@
       <c r="Y6" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="Z6" s="10"/>
+      <c r="Z6" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA6" s="20" t="s">
+        <v>169</v>
+      </c>
       <c r="AB6"/>
       <c r="AC6"/>
       <c r="AE6" s="20"/>
@@ -1364,7 +1384,12 @@
       <c r="Y7" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="Z7" s="10"/>
+      <c r="Z7" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA7" s="20" t="s">
+        <v>170</v>
+      </c>
       <c r="AB7"/>
       <c r="AC7"/>
       <c r="AE7" s="20"/>
@@ -1430,7 +1455,9 @@
       <c r="Y8" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="Z8" s="10"/>
+      <c r="Z8" s="20" t="s">
+        <v>168</v>
+      </c>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
       <c r="AE8" s="20"/>

</xml_diff>

<commit_message>
datamodel og iterationsplan opdateret
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/proj. mgt/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/proj. mgt/Iteration og faseplan.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bloms\OneDrive\Dokumenter\GitHub\FFT\modeller, dokumenter\proj. mgt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_F2EF9CF74CFB6915D7931668D0B9294EDAF850A0" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{14FCCA57-1252-4A96-B7E6-1C391C2CAE6C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overordnet projektplan" sheetId="1" r:id="rId1"/>
     <sheet name="Milepæle" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="172">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -533,13 +539,16 @@
   </si>
   <si>
     <t>implementation af UC5</t>
+  </si>
+  <si>
+    <t>implementere detaljer i GUI-klasse og datalayer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -970,60 +979,59 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Ark1"/>
-  <dimension ref="A1:AH44"/>
+  <dimension ref="A1:AG44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AA8" sqref="AA8"/>
+      <selection pane="bottomRight" activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="43" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="10" customWidth="1"/>
-    <col min="14" max="14" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" style="10" customWidth="1"/>
+    <col min="14" max="14" width="35.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.28515625" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.33203125" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="35" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.28515625" customWidth="1"/>
-    <col min="24" max="24" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="35.28515625" style="10" customWidth="1"/>
-    <col min="30" max="30" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="34" width="28.7109375" customWidth="1"/>
+    <col min="22" max="22" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.33203125" customWidth="1"/>
+    <col min="24" max="24" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="40.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="33" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="11" customFormat="1" ht="18.75">
+    <row r="1" spans="1:33" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
@@ -1047,12 +1055,11 @@
       </c>
       <c r="AA1" s="16"/>
       <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="18" customFormat="1">
+    <row r="2" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>15</v>
       </c>
@@ -1073,12 +1080,11 @@
         <v>10</v>
       </c>
       <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="17" t="s">
+      <c r="AC2" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:34" s="5" customFormat="1">
+    <row r="3" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -1143,28 +1149,25 @@
         <v>43244</v>
       </c>
       <c r="AB3" s="3">
-        <v>43244</v>
+        <v>43245</v>
       </c>
       <c r="AC3" s="3">
-        <v>43245</v>
+        <v>43248</v>
       </c>
       <c r="AD3" s="3">
-        <v>43248</v>
+        <v>43249</v>
       </c>
       <c r="AE3" s="3">
-        <v>43249</v>
+        <v>43250</v>
       </c>
       <c r="AF3" s="3">
-        <v>43250</v>
+        <v>43251</v>
       </c>
       <c r="AG3" s="3">
-        <v>43251</v>
-      </c>
-      <c r="AH3" s="3">
         <v>43252</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
@@ -1220,10 +1223,10 @@
       <c r="AB4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="AC4" s="10" t="s">
+      <c r="AC4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AD4" t="s">
         <v>3</v>
       </c>
       <c r="AE4" t="s">
@@ -1235,15 +1238,12 @@
       <c r="AG4" t="s">
         <v>3</v>
       </c>
-      <c r="AH4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34">
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1316,16 +1316,17 @@
       <c r="AA6" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="AB6"/>
-      <c r="AC6"/>
+      <c r="AB6" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
       <c r="AF6" s="20"/>
-      <c r="AG6" s="20"/>
-      <c r="AH6" s="20" t="s">
+      <c r="AG6" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1390,14 +1391,15 @@
       <c r="AA7" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="AB7"/>
-      <c r="AC7"/>
+      <c r="AB7" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
       <c r="AF7" s="20"/>
       <c r="AG7" s="20"/>
-      <c r="AH7" s="20"/>
-    </row>
-    <row r="8" spans="1:34">
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1459,13 +1461,12 @@
         <v>168</v>
       </c>
       <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
+      <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
       <c r="AF8" s="20"/>
       <c r="AG8" s="20"/>
-      <c r="AH8" s="20"/>
-    </row>
-    <row r="9" spans="1:34">
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1527,10 +1528,9 @@
       </c>
       <c r="Z9" s="10"/>
       <c r="AB9" s="8"/>
-      <c r="AC9" s="8"/>
-      <c r="AD9" s="9"/>
-    </row>
-    <row r="10" spans="1:34">
+      <c r="AC9" s="9"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1575,13 +1575,12 @@
       </c>
       <c r="Z10" s="10"/>
       <c r="AB10" s="8"/>
-      <c r="AC10" s="8"/>
+      <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
       <c r="AG10" s="20"/>
-      <c r="AH10" s="20"/>
-    </row>
-    <row r="11" spans="1:34">
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>39</v>
       </c>
@@ -1612,9 +1611,8 @@
       <c r="Y11" s="9"/>
       <c r="Z11" s="10"/>
       <c r="AB11" s="8"/>
-      <c r="AC11" s="8"/>
-    </row>
-    <row r="12" spans="1:34">
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>35</v>
       </c>
@@ -1632,13 +1630,12 @@
       </c>
       <c r="Z12" s="10"/>
       <c r="AB12" s="8"/>
-      <c r="AC12" s="8"/>
+      <c r="AD12" s="7"/>
       <c r="AE12" s="7"/>
       <c r="AF12" s="7"/>
       <c r="AG12" s="7"/>
-      <c r="AH12" s="7"/>
-    </row>
-    <row r="13" spans="1:34">
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>36</v>
       </c>
@@ -1661,13 +1658,12 @@
       <c r="O13" s="10"/>
       <c r="Z13" s="10"/>
       <c r="AB13" s="8"/>
-      <c r="AC13" s="8"/>
+      <c r="AD13" s="8"/>
       <c r="AE13" s="8"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8"/>
-      <c r="AH13" s="8"/>
-    </row>
-    <row r="14" spans="1:34">
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="J14" s="1" t="s">
         <v>66</v>
       </c>
@@ -1680,13 +1676,12 @@
       <c r="O14" s="10"/>
       <c r="Z14" s="10"/>
       <c r="AB14" s="8"/>
-      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
       <c r="AF14" s="8"/>
       <c r="AG14" s="8"/>
-      <c r="AH14" s="8"/>
-    </row>
-    <row r="15" spans="1:34">
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1698,7 +1693,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -1708,7 +1703,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="4:24">
+    <row r="17" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1719,7 +1714,7 @@
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
     </row>
-    <row r="18" spans="4:24">
+    <row r="18" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1730,7 +1725,7 @@
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
     </row>
-    <row r="19" spans="4:24">
+    <row r="19" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1743,7 +1738,7 @@
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
     </row>
-    <row r="20" spans="4:24">
+    <row r="20" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1756,7 +1751,7 @@
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
     </row>
-    <row r="21" spans="4:24">
+    <row r="21" spans="4:24" x14ac:dyDescent="0.3">
       <c r="D21" s="8"/>
       <c r="I21" s="1"/>
       <c r="L21"/>
@@ -1766,7 +1761,7 @@
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="4:24">
+    <row r="22" spans="4:24" x14ac:dyDescent="0.3">
       <c r="H22" s="8"/>
       <c r="I22" s="1"/>
       <c r="L22"/>
@@ -1779,7 +1774,7 @@
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
     </row>
-    <row r="23" spans="4:24">
+    <row r="23" spans="4:24" x14ac:dyDescent="0.3">
       <c r="H23" s="8"/>
       <c r="I23" s="1"/>
       <c r="L23"/>
@@ -1792,7 +1787,7 @@
       <c r="W23" s="8"/>
       <c r="X23" s="8"/>
     </row>
-    <row r="24" spans="4:24">
+    <row r="24" spans="4:24" x14ac:dyDescent="0.3">
       <c r="H24" s="8"/>
       <c r="I24" s="1"/>
       <c r="L24"/>
@@ -1805,7 +1800,7 @@
       <c r="W24" s="8"/>
       <c r="X24" s="8"/>
     </row>
-    <row r="25" spans="4:24">
+    <row r="25" spans="4:24" x14ac:dyDescent="0.3">
       <c r="H25" s="8"/>
       <c r="I25" s="1"/>
       <c r="T25" s="2"/>
@@ -1813,21 +1808,21 @@
       <c r="W25" s="8"/>
       <c r="X25" s="8"/>
     </row>
-    <row r="26" spans="4:24">
+    <row r="26" spans="4:24" x14ac:dyDescent="0.3">
       <c r="I26" s="1"/>
       <c r="T26" s="2"/>
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
       <c r="X26" s="8"/>
     </row>
-    <row r="27" spans="4:24">
+    <row r="27" spans="4:24" x14ac:dyDescent="0.3">
       <c r="I27" s="1"/>
       <c r="T27" s="2"/>
       <c r="V27" s="8"/>
       <c r="W27" s="8"/>
       <c r="X27" s="8"/>
     </row>
-    <row r="28" spans="4:24">
+    <row r="28" spans="4:24" x14ac:dyDescent="0.3">
       <c r="I28" s="1"/>
       <c r="T28" s="2" t="s">
         <v>122</v>
@@ -1836,7 +1831,7 @@
       <c r="W28" s="8"/>
       <c r="X28" s="8"/>
     </row>
-    <row r="29" spans="4:24">
+    <row r="29" spans="4:24" x14ac:dyDescent="0.3">
       <c r="I29" s="1"/>
       <c r="K29" s="14"/>
       <c r="T29" s="2"/>
@@ -1844,7 +1839,7 @@
       <c r="W29" s="8"/>
       <c r="X29" s="8"/>
     </row>
-    <row r="30" spans="4:24">
+    <row r="30" spans="4:24" x14ac:dyDescent="0.3">
       <c r="I30" s="2"/>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
@@ -1856,7 +1851,7 @@
       <c r="W30" s="8"/>
       <c r="X30" s="8"/>
     </row>
-    <row r="31" spans="4:24">
+    <row r="31" spans="4:24" x14ac:dyDescent="0.3">
       <c r="I31" s="2"/>
       <c r="K31" s="14"/>
       <c r="T31" s="2" t="s">
@@ -1866,7 +1861,7 @@
       <c r="W31" s="8"/>
       <c r="X31" s="8"/>
     </row>
-    <row r="32" spans="4:24">
+    <row r="32" spans="4:24" x14ac:dyDescent="0.3">
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="K32" s="14"/>
@@ -1876,7 +1871,7 @@
       <c r="W32" s="8"/>
       <c r="X32" s="8"/>
     </row>
-    <row r="33" spans="8:24">
+    <row r="33" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="K33" s="14"/>
@@ -1884,7 +1879,7 @@
       <c r="W33" s="8"/>
       <c r="X33" s="8"/>
     </row>
-    <row r="34" spans="8:24">
+    <row r="34" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="K34" s="14"/>
@@ -1892,7 +1887,7 @@
       <c r="W34" s="8"/>
       <c r="X34" s="8"/>
     </row>
-    <row r="35" spans="8:24">
+    <row r="35" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="K35" s="14"/>
@@ -1900,25 +1895,25 @@
       <c r="W35" s="8"/>
       <c r="X35" s="8"/>
     </row>
-    <row r="36" spans="8:24">
+    <row r="36" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="8:24">
+    <row r="37" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="8:24">
+    <row r="38" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H38" s="2"/>
     </row>
-    <row r="41" spans="8:24">
+    <row r="41" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="8:24">
+    <row r="42" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="8:24">
+    <row r="43" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="8:24">
+    <row r="44" spans="8:24" x14ac:dyDescent="0.3">
       <c r="H44" s="8"/>
     </row>
   </sheetData>
@@ -1928,7 +1923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Ark2"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -1939,19 +1934,19 @@
       <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" customWidth="1"/>
-    <col min="7" max="7" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="6"/>
+    <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.33203125" customWidth="1"/>
+    <col min="7" max="7" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" ht="18.75">
+    <row r="1" spans="1:8" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
@@ -1968,7 +1963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="12" customFormat="1">
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>15</v>
       </c>
@@ -1994,7 +1989,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>52</v>
       </c>
@@ -2016,7 +2011,7 @@
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>96</v>
       </c>
@@ -2035,7 +2030,7 @@
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>97</v>
       </c>
@@ -2054,7 +2049,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>103</v>
       </c>
@@ -2073,7 +2068,7 @@
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>99</v>
       </c>
@@ -2092,7 +2087,7 @@
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>100</v>
       </c>
@@ -2111,7 +2106,7 @@
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>102</v>
       </c>
@@ -2130,7 +2125,7 @@
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>101</v>
       </c>
@@ -2146,7 +2141,7 @@
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>104</v>
       </c>
@@ -2159,7 +2154,7 @@
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>109</v>
       </c>
@@ -2169,29 +2164,29 @@
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>84</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>110</v>
       </c>
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>1</v>
       </c>
@@ -2208,7 +2203,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>28</v>
       </c>
@@ -2222,7 +2217,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>27</v>
       </c>
@@ -2236,7 +2231,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
         <v>29</v>
       </c>
@@ -2244,7 +2239,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
opdatering af diagrammer og bilag
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/proj. mgt/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/proj. mgt/Iteration og faseplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bloms\OneDrive\Dokumenter\GitHub\FFT\modeller, dokumenter\proj. mgt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_F2EF9CF74CFB6915D7931668D0B9294EDAF850A0" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{14FCCA57-1252-4A96-B7E6-1C391C2CAE6C}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_F2EF9CF74CFB6915D7931668D0B9294EDAF850A0" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{33A8F7F8-0C70-4269-89D2-2121B093F040}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overordnet projektplan" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="176">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Iteration E2</t>
   </si>
   <si>
-    <t>Iteration C3</t>
-  </si>
-  <si>
     <t>Iterationsplan for E1 er klar</t>
   </si>
   <si>
@@ -82,9 +79,6 @@
     <t>Dato</t>
   </si>
   <si>
-    <t>Iteration T4</t>
-  </si>
-  <si>
     <t>Udarbejdelse af faseplan</t>
   </si>
   <si>
@@ -457,9 +451,6 @@
     <t>Unit test af UC3</t>
   </si>
   <si>
-    <t>E4 28/5 - 1/5</t>
-  </si>
-  <si>
     <t>Tests (System-, Accept-, Integrations-)</t>
   </si>
   <si>
@@ -542,6 +533,27 @@
   </si>
   <si>
     <t>implementere detaljer i GUI-klasse og datalayer</t>
+  </si>
+  <si>
+    <t>Iteration E3</t>
+  </si>
+  <si>
+    <t>Iteration E4</t>
+  </si>
+  <si>
+    <t>genimplementation af UC5</t>
+  </si>
+  <si>
+    <t>kommentarer i kode</t>
+  </si>
+  <si>
+    <t>gennemgang af kode</t>
+  </si>
+  <si>
+    <t>opdatere klassediagram</t>
+  </si>
+  <si>
+    <t>E4 28/5 - 1/6</t>
   </si>
 </sst>
 </file>
@@ -990,11 +1002,11 @@
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AG44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="AA4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="AB4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AB8" sqref="AB8"/>
+      <selection pane="bottomRight" activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1033,7 +1045,7 @@
   <sheetData>
     <row r="1" spans="1:33" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>4</v>
@@ -1050,21 +1062,17 @@
       <c r="R1" s="16"/>
       <c r="S1" s="16"/>
       <c r="T1" s="15"/>
-      <c r="Y1" s="15" t="s">
-        <v>6</v>
-      </c>
+      <c r="Y1" s="15"/>
       <c r="AA1" s="16"/>
       <c r="AB1" s="16"/>
-      <c r="AC1" s="15" t="s">
-        <v>7</v>
-      </c>
+      <c r="AC1" s="15"/>
     </row>
     <row r="2" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="19"/>
       <c r="J2" s="17" t="s">
@@ -1077,16 +1085,16 @@
         <v>9</v>
       </c>
       <c r="Y2" s="17" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="AB2" s="19"/>
       <c r="AC2" s="17" t="s">
-        <v>18</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4">
         <v>43220</v>
@@ -1169,7 +1177,7 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -1245,222 +1253,237 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H6" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="20" t="s">
-        <v>50</v>
-      </c>
       <c r="L6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="M6" s="20" t="s">
-        <v>70</v>
-      </c>
       <c r="N6" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="P6" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="O6" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="P6" s="20" t="s">
-        <v>81</v>
-      </c>
       <c r="Q6" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="R6" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="U6" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="S6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="T6" s="1" t="s">
+      <c r="V6" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="W6" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="X6" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z6" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA6" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB6" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="U6" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="V6" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="W6" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="X6" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="Z6" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA6" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="AB6" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD6" s="20"/>
-      <c r="AE6" s="20"/>
+      <c r="AC6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD6" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE6" s="20" t="s">
+        <v>174</v>
+      </c>
       <c r="AF6" s="20"/>
       <c r="AG6" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q7" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
       <c r="T7" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="V7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="W7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="Y7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z7" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="Z7" s="20" t="s">
-        <v>166</v>
-      </c>
       <c r="AA7" s="20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="AB7" s="20" t="s">
-        <v>171</v>
+        <v>168</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="AD7" s="20"/>
-      <c r="AE7" s="20"/>
+      <c r="AE7" s="20" t="s">
+        <v>122</v>
+      </c>
       <c r="AF7" s="20"/>
       <c r="AG7" s="20"/>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="Q8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T8" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="U8" t="s">
+        <v>119</v>
+      </c>
+      <c r="V8" t="s">
         <v>126</v>
       </c>
-      <c r="U8" t="s">
-        <v>121</v>
-      </c>
-      <c r="V8" t="s">
-        <v>128</v>
-      </c>
       <c r="W8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Z8" s="20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="AB8" s="7"/>
+      <c r="AC8" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
       <c r="AF8" s="20"/>
@@ -1468,63 +1491,63 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F9" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="20" t="s">
-        <v>46</v>
-      </c>
       <c r="H9" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="K9" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>61</v>
-      </c>
       <c r="L9" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="U9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="V9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="W9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="Z9" s="10"/>
       <c r="AB9" s="8"/>
@@ -1532,46 +1555,46 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="U10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="V10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W10" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Z10" s="10"/>
       <c r="AB10" s="8"/>
@@ -1582,31 +1605,31 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L11" s="20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="V11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="Y11" s="9"/>
       <c r="Z11" s="10"/>
@@ -1614,19 +1637,19 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Z12" s="10"/>
       <c r="AB12" s="8"/>
@@ -1637,22 +1660,22 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L13" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1665,10 +1688,10 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="J14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L14"/>
       <c r="M14"/>
@@ -1687,10 +1710,10 @@
       <c r="G15" s="7"/>
       <c r="I15" s="9"/>
       <c r="J15" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
@@ -1700,7 +1723,7 @@
       <c r="G16" s="8"/>
       <c r="I16" s="1"/>
       <c r="U16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="4:24" x14ac:dyDescent="0.3">
@@ -1825,7 +1848,7 @@
     <row r="28" spans="4:24" x14ac:dyDescent="0.3">
       <c r="I28" s="1"/>
       <c r="T28" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="V28" s="8"/>
       <c r="W28" s="8"/>
@@ -1845,7 +1868,7 @@
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
       <c r="T30" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="V30" s="8"/>
       <c r="W30" s="8"/>
@@ -1855,7 +1878,7 @@
       <c r="I31" s="2"/>
       <c r="K31" s="14"/>
       <c r="T31" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="V31" s="8"/>
       <c r="W31" s="8"/>
@@ -1927,11 +1950,11 @@
   <sheetPr codeName="Ark2"/>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" sqref="A1:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1940,7 +1963,7 @@
     <col min="2" max="2" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="40.33203125" customWidth="1"/>
     <col min="7" max="7" width="42.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.44140625" bestFit="1" customWidth="1"/>
@@ -1948,7 +1971,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>4</v>
@@ -1965,215 +1988,215 @@
     </row>
     <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="G2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>12</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
@@ -2194,54 +2217,54 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="23" t="s">
-        <v>90</v>
-      </c>
       <c r="H17" s="23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H18" s="23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H19" s="23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>